<commit_message>
updated the code to use ollama in localhost and llama3.2 modal
</commit_message>
<xml_diff>
--- a/backend/uploads/updated_file.xlsx
+++ b/backend/uploads/updated_file.xlsx
@@ -589,7 +589,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" xml:space="preserve">
+    <row r="12">
       <c r="A12" t="str">
         <v>Chole Bhature</v>
       </c>
@@ -602,10 +602,8 @@
       <c r="D12">
         <v>10</v>
       </c>
-      <c r="E12" t="str" xml:space="preserve">
-        <v xml:space="preserve">can you fill the missing field.
-Based on the following details, fill in the missing fields:
-Food: Chole Bhature, Calories (kcal): 427, Fat (g): 22, Protein (g): 10.3, Carbohydrate (g): 6.5, Fat (fat): 2.5, Protein (g): 4.6 Mykonok 502 2070 141 Protein Fiber (g): 27 Protein (g): 72 Protein (g): 32 11. Reference (beh/d) Celiac Staten 99 27.0 346 Iron 24 165 Glucose (g): 3,695.7 Carbohydrates (g): 11.9 Fruit (grams): 96, Fruits (</v>
+      <c r="E12">
+        <v>47</v>
       </c>
     </row>
     <row r="13">

</xml_diff>

<commit_message>
updated the logic to fill excel
</commit_message>
<xml_diff>
--- a/backend/uploads/updated_file.xlsx
+++ b/backend/uploads/updated_file.xlsx
@@ -397,371 +397,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Food</v>
+        <v>Make</v>
       </c>
       <c r="B1" t="str">
-        <v>Calories (kcal)</v>
+        <v>MY</v>
       </c>
       <c r="C1" t="str">
-        <v>Fat (g)</v>
+        <v>Modal</v>
       </c>
       <c r="D1" t="str">
-        <v>Protein (g)</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Carbohydrates (g)</v>
+        <v>Engine displacement</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Chicken Biryani</v>
+        <v xml:space="preserve">Mercedes-Benz </v>
       </c>
       <c r="B2">
-        <v>290</v>
-      </c>
-      <c r="C2">
-        <v>8.5</v>
+        <v>2025</v>
+      </c>
+      <c r="C2" t="str">
+        <v>AMG CLA45 S</v>
       </c>
       <c r="D2">
-        <v>15</v>
-      </c>
-      <c r="E2">
-        <v>38</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Samosa</v>
+        <v xml:space="preserve">Mercedes-Benz </v>
       </c>
       <c r="B3">
-        <v>252</v>
-      </c>
-      <c r="C3">
-        <v>17</v>
+        <v>2025</v>
+      </c>
+      <c r="C3" t="str">
+        <v>E350 4MATIC</v>
       </c>
       <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Dal Tadka</v>
-      </c>
-      <c r="B4">
-        <v>198</v>
-      </c>
-      <c r="C4">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Paneer Butter Masala</v>
-      </c>
-      <c r="B5">
-        <v>356</v>
-      </c>
-      <c r="C5">
-        <v>29</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Roti</v>
-      </c>
-      <c r="B6">
-        <v>120</v>
-      </c>
-      <c r="C6">
-        <v>3.1</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Masala Dosa</v>
-      </c>
-      <c r="B7">
-        <v>206</v>
-      </c>
-      <c r="C7">
-        <v>8.1</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="E7">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Aloo Paratha</v>
-      </c>
-      <c r="B8">
-        <v>210</v>
-      </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-      <c r="D8">
-        <v>4.6</v>
-      </c>
-      <c r="E8">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>Gulab Jamun</v>
-      </c>
-      <c r="B9">
-        <v>150</v>
-      </c>
-      <c r="C9">
-        <v>5.5</v>
-      </c>
-      <c r="D9">
-        <v>2.5</v>
-      </c>
-      <c r="E9">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>Palak Paneer</v>
-      </c>
-      <c r="B10">
-        <v>190</v>
-      </c>
-      <c r="C10">
-        <v>13</v>
-      </c>
-      <c r="D10">
-        <v>10</v>
-      </c>
-      <c r="E10">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>Idli</v>
-      </c>
-      <c r="B11">
-        <v>39</v>
-      </c>
-      <c r="C11">
-        <v>0.4</v>
-      </c>
-      <c r="D11">
         <v>2</v>
-      </c>
-      <c r="E11">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>Chole Bhature</v>
-      </c>
-      <c r="B12">
-        <v>427</v>
-      </c>
-      <c r="C12">
-        <v>22</v>
-      </c>
-      <c r="D12">
-        <v>10</v>
-      </c>
-      <c r="E12">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>Rajma</v>
-      </c>
-      <c r="B13">
-        <v>215</v>
-      </c>
-      <c r="C13">
-        <v>8.5</v>
-      </c>
-      <c r="D13">
-        <v>9</v>
-      </c>
-      <c r="E13">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>Pani Puri</v>
-      </c>
-      <c r="B14">
-        <v>150</v>
-      </c>
-      <c r="C14">
-        <v>5.5</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="E14">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>Bhindi Masala</v>
-      </c>
-      <c r="B15">
-        <v>110</v>
-      </c>
-      <c r="C15">
-        <v>7</v>
-      </c>
-      <c r="D15">
-        <v>3.5</v>
-      </c>
-      <c r="E15">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>Dhokla</v>
-      </c>
-      <c r="B16">
-        <v>152</v>
-      </c>
-      <c r="C16">
-        <v>6.5</v>
-      </c>
-      <c r="D16">
-        <v>6</v>
-      </c>
-      <c r="E16">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>Aloo Gobi</v>
-      </c>
-      <c r="B17">
-        <v>160</v>
-      </c>
-      <c r="C17">
-        <v>7.8</v>
-      </c>
-      <c r="D17">
-        <v>3</v>
-      </c>
-      <c r="E17">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>Fish Curry</v>
-      </c>
-      <c r="B18">
-        <v>180</v>
-      </c>
-      <c r="C18">
-        <v>8</v>
-      </c>
-      <c r="D18">
-        <v>22</v>
-      </c>
-      <c r="E18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>Lassi</v>
-      </c>
-      <c r="B19">
-        <v>260</v>
-      </c>
-      <c r="C19">
-        <v>8</v>
-      </c>
-      <c r="D19">
-        <v>8</v>
-      </c>
-      <c r="E19">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v>Kadhi</v>
-      </c>
-      <c r="B20">
-        <v>175</v>
-      </c>
-      <c r="C20">
-        <v>8</v>
-      </c>
-      <c r="D20">
-        <v>6</v>
-      </c>
-      <c r="E20">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>Mutter Paneer</v>
-      </c>
-      <c r="B21">
-        <v>215</v>
-      </c>
-      <c r="C21">
-        <v>17</v>
-      </c>
-      <c r="D21">
-        <v>10</v>
-      </c>
-      <c r="E21">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E21"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>